<commit_message>
ÂImplemented ai and error text colouring to help users debug invalid emails
</commit_message>
<xml_diff>
--- a/spreadsheets/valid_test.xlsx
+++ b/spreadsheets/valid_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ra1422_ic_ac_uk/Documents/extra work/projects/python/email-client/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D0A1480-2D93-4A48-B4CF-B950D21C014A}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21E4E87F-504D-4492-B5E6-EBCAF4668E3B}"/>
   <bookViews>
     <workbookView xWindow="5004" yWindow="1032" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Company name</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>test_template_1.docx</t>
+  </si>
+  <si>
+    <t>Company F</t>
+  </si>
+  <si>
+    <t>Something Else</t>
+  </si>
+  <si>
+    <t>ai_email@gmail.com</t>
+  </si>
+  <si>
+    <t>file_for_ai.txt</t>
+  </si>
+  <si>
+    <t>rayanakhtar1203@gmail.com</t>
+  </si>
+  <si>
+    <t>AI internship</t>
+  </si>
+  <si>
+    <t>ai_template_1.txt</t>
   </si>
 </sst>
 </file>
@@ -450,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,6 +607,29 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{49F97E77-A62C-4415-8FB2-DF13A8600D23}"/>
@@ -596,6 +640,8 @@
     <hyperlink ref="F4" r:id="rId6" xr:uid="{91BDD6F1-2B7E-45EA-B5AE-0A94D9F524B6}"/>
     <hyperlink ref="D6" r:id="rId7" xr:uid="{F473D3A3-A6D8-45FD-8023-DBBAD9373CE5}"/>
     <hyperlink ref="F6" r:id="rId8" xr:uid="{5B36796B-F14F-440A-98A4-200F019677ED}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{A8738982-210D-4129-B2DB-E191FAAB8AD9}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{A0CFCE14-8D6A-4FFF-97F5-73D43766ABB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>